<commit_message>
cambio de primera clasificacion
</commit_message>
<xml_diff>
--- a/sys/cla/files/claara/tplClasificacionMercancias.xlsx
+++ b/sys/cla/files/claara/tplClasificacionMercancias.xlsx
@@ -1,24 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\VBOXSVR\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28095" windowHeight="12330"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -27,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>REFERENCIA</t>
   </si>
   <si>
-    <t>PEDIMENTO</t>
-  </si>
-  <si>
-    <t>CLIENTE</t>
-  </si>
-  <si>
     <t>DESCRIPCION</t>
   </si>
   <si>
@@ -50,19 +42,10 @@
     <t>FACTURA</t>
   </si>
   <si>
-    <t>AUTOR</t>
-  </si>
-  <si>
     <t>FRACCION</t>
   </si>
   <si>
     <t>F DE PREVIO</t>
-  </si>
-  <si>
-    <t>CONSECUTIVO</t>
-  </si>
-  <si>
-    <t>REGIMEN</t>
   </si>
 </sst>
 </file>
@@ -176,7 +159,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -211,7 +194,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -388,7 +371,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -396,68 +379,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L1"/>
+  <autoFilter ref="A1:G1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>